<commit_message>
Kommentar für Ergebnis wieder auskommentiert
</commit_message>
<xml_diff>
--- a/Python Comparer/comparison_results.xlsx
+++ b/Python Comparer/comparison_results.xlsx
@@ -445,16 +445,16 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-2147483648</v>
+        <v>2147483600</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertachtundvierzig</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundert</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertachtundvierzig</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundert</t>
         </is>
       </c>
       <c r="D2" t="b">
@@ -463,16 +463,16 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>-2147483647</v>
+        <v>2147483601</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertsiebenundvierzig</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshunderteins</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertsiebenundvierzig</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshunderteins</t>
         </is>
       </c>
       <c r="D3" t="b">
@@ -481,16 +481,16 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>-2147483646</v>
+        <v>2147483602</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertsechsundvierzig</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertzwei</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertsechsundvierzig</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertzwei</t>
         </is>
       </c>
       <c r="D4" t="b">
@@ -499,16 +499,16 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>-2147483645</v>
+        <v>2147483603</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertfuenfundvierzig</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertdrei</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertfuenfundvierzig</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertdrei</t>
         </is>
       </c>
       <c r="D5" t="b">
@@ -517,16 +517,16 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>-2147483644</v>
+        <v>2147483604</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertvierundvierzig</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertvier</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertvierundvierzig</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertvier</t>
         </is>
       </c>
       <c r="D6" t="b">
@@ -535,16 +535,16 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>-2147483643</v>
+        <v>2147483605</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertdreiundvierzig</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertfuenf</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertdreiundvierzig</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertfuenf</t>
         </is>
       </c>
       <c r="D7" t="b">
@@ -553,16 +553,16 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>-2147483642</v>
+        <v>2147483606</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertzweiundvierzig</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertsechs</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertzweiundvierzig</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertsechs</t>
         </is>
       </c>
       <c r="D8" t="b">
@@ -571,16 +571,16 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>-2147483641</v>
+        <v>2147483607</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshunderteinundvierzig</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertsieben</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshunderteinundvierzig</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertsieben</t>
         </is>
       </c>
       <c r="D9" t="b">
@@ -589,16 +589,16 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>-2147483640</v>
+        <v>2147483608</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertvierzig</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertacht</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertvierzig</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertacht</t>
         </is>
       </c>
       <c r="D10" t="b">
@@ -607,16 +607,16 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>-2147483639</v>
+        <v>2147483609</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertneununddreissig</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertneun</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertneununddreissig</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertneun</t>
         </is>
       </c>
       <c r="D11" t="b">
@@ -625,16 +625,16 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>-2147483638</v>
+        <v>2147483610</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertachtunddreissig</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertzehn</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertachtunddreissig</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertzehn</t>
         </is>
       </c>
       <c r="D12" t="b">
@@ -643,16 +643,16 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>-2147483637</v>
+        <v>2147483611</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertsiebenunddreissig</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertelf</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertsiebenunddreissig</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertelf</t>
         </is>
       </c>
       <c r="D13" t="b">
@@ -661,16 +661,16 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>-2147483636</v>
+        <v>2147483612</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertsechsunddreissig</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertzwoelf</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertsechsunddreissig</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertzwoelf</t>
         </is>
       </c>
       <c r="D14" t="b">
@@ -679,16 +679,16 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>-2147483635</v>
+        <v>2147483613</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertfuenfunddreissig</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertdreizehn</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertfuenfunddreissig</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertdreizehn</t>
         </is>
       </c>
       <c r="D15" t="b">
@@ -697,16 +697,16 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>-2147483634</v>
+        <v>2147483614</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertvierunddreissig</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertvierzehn</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertvierunddreissig</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertvierzehn</t>
         </is>
       </c>
       <c r="D16" t="b">
@@ -715,16 +715,16 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>-2147483633</v>
+        <v>2147483615</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertdreiunddreissig</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertfuenfzehn</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertdreiunddreissig</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertfuenfzehn</t>
         </is>
       </c>
       <c r="D17" t="b">
@@ -733,16 +733,16 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>-2147483632</v>
+        <v>2147483616</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertzweiunddreissig</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertsechzehn</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertzweiunddreissig</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertsechzehn</t>
         </is>
       </c>
       <c r="D18" t="b">
@@ -751,16 +751,16 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>-2147483631</v>
+        <v>2147483617</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshunderteinunddreissig</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertsiebzehn</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshunderteinunddreissig</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertsiebzehn</t>
         </is>
       </c>
       <c r="D19" t="b">
@@ -769,16 +769,16 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>-2147483630</v>
+        <v>2147483618</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertdreissig</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertachtzehn</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertdreissig</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertachtzehn</t>
         </is>
       </c>
       <c r="D20" t="b">
@@ -787,16 +787,16 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>-2147483629</v>
+        <v>2147483619</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertneunundzwanzig</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertneunzehn</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertneunundzwanzig</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertneunzehn</t>
         </is>
       </c>
       <c r="D21" t="b">
@@ -805,16 +805,16 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>-2147483628</v>
+        <v>2147483620</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertachtundzwanzig</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertzwanzig</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertachtundzwanzig</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertzwanzig</t>
         </is>
       </c>
       <c r="D22" t="b">
@@ -823,16 +823,16 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>-2147483627</v>
+        <v>2147483621</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertsiebenundzwanzig</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshunderteinundzwanzig</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertsiebenundzwanzig</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshunderteinundzwanzig</t>
         </is>
       </c>
       <c r="D23" t="b">
@@ -841,16 +841,16 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>-2147483626</v>
+        <v>2147483622</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertsechsundzwanzig</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertzweiundzwanzig</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertsechsundzwanzig</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertzweiundzwanzig</t>
         </is>
       </c>
       <c r="D24" t="b">
@@ -859,16 +859,16 @@
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>-2147483625</v>
+        <v>2147483623</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertfuenfundzwanzig</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertdreiundzwanzig</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertfuenfundzwanzig</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertdreiundzwanzig</t>
         </is>
       </c>
       <c r="D25" t="b">
@@ -877,16 +877,16 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>-2147483624</v>
+        <v>2147483624</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertvierundzwanzig</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertvierundzwanzig</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertvierundzwanzig</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertvierundzwanzig</t>
         </is>
       </c>
       <c r="D26" t="b">
@@ -895,16 +895,16 @@
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>-2147483623</v>
+        <v>2147483625</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertdreiundzwanzig</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertfuenfundzwanzig</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertdreiundzwanzig</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertfuenfundzwanzig</t>
         </is>
       </c>
       <c r="D27" t="b">
@@ -913,16 +913,16 @@
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>-2147483622</v>
+        <v>2147483626</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertzweiundzwanzig</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertsechsundzwanzig</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertzweiundzwanzig</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertsechsundzwanzig</t>
         </is>
       </c>
       <c r="D28" t="b">
@@ -931,16 +931,16 @@
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>-2147483621</v>
+        <v>2147483627</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshunderteinundzwanzig</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertsiebenundzwanzig</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshunderteinundzwanzig</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertsiebenundzwanzig</t>
         </is>
       </c>
       <c r="D29" t="b">
@@ -949,16 +949,16 @@
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>-2147483620</v>
+        <v>2147483628</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertzwanzig</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertachtundzwanzig</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertzwanzig</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertachtundzwanzig</t>
         </is>
       </c>
       <c r="D30" t="b">
@@ -967,16 +967,16 @@
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>-2147483619</v>
+        <v>2147483629</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertneunzehn</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertneunundzwanzig</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertneunzehn</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertneunundzwanzig</t>
         </is>
       </c>
       <c r="D31" t="b">
@@ -985,16 +985,16 @@
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>-2147483618</v>
+        <v>2147483630</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertachtzehn</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertdreissig</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertachtzehn</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertdreissig</t>
         </is>
       </c>
       <c r="D32" t="b">
@@ -1003,16 +1003,16 @@
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>-2147483617</v>
+        <v>2147483631</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertsiebzehn</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshunderteinunddreissig</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertsiebzehn</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshunderteinunddreissig</t>
         </is>
       </c>
       <c r="D33" t="b">
@@ -1021,16 +1021,16 @@
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>-2147483616</v>
+        <v>2147483632</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertsechzehn</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertzweiunddreissig</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertsechzehn</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertzweiunddreissig</t>
         </is>
       </c>
       <c r="D34" t="b">
@@ -1039,16 +1039,16 @@
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>-2147483615</v>
+        <v>2147483633</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertfuenfzehn</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertdreiunddreissig</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertfuenfzehn</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertdreiunddreissig</t>
         </is>
       </c>
       <c r="D35" t="b">
@@ -1057,16 +1057,16 @@
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>-2147483614</v>
+        <v>2147483634</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertvierzehn</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertvierunddreissig</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertvierzehn</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertvierunddreissig</t>
         </is>
       </c>
       <c r="D36" t="b">
@@ -1075,16 +1075,16 @@
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>-2147483613</v>
+        <v>2147483635</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertdreizehn</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertfuenfunddreissig</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertdreizehn</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertfuenfunddreissig</t>
         </is>
       </c>
       <c r="D37" t="b">
@@ -1093,16 +1093,16 @@
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>-2147483612</v>
+        <v>2147483636</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertzwoelf</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertsechsunddreissig</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertzwoelf</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertsechsunddreissig</t>
         </is>
       </c>
       <c r="D38" t="b">
@@ -1111,16 +1111,16 @@
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>-2147483611</v>
+        <v>2147483637</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertelf</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertsiebenunddreissig</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertelf</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertsiebenunddreissig</t>
         </is>
       </c>
       <c r="D39" t="b">
@@ -1129,16 +1129,16 @@
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>-2147483610</v>
+        <v>2147483638</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertzehn</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertachtunddreissig</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertzehn</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertachtunddreissig</t>
         </is>
       </c>
       <c r="D40" t="b">
@@ -1147,16 +1147,16 @@
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>-2147483609</v>
+        <v>2147483639</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertneun</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertneununddreissig</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertneun</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertneununddreissig</t>
         </is>
       </c>
       <c r="D41" t="b">
@@ -1165,16 +1165,16 @@
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>-2147483608</v>
+        <v>2147483640</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertacht</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertvierzig</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertacht</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertvierzig</t>
         </is>
       </c>
       <c r="D42" t="b">
@@ -1183,16 +1183,16 @@
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>-2147483607</v>
+        <v>2147483641</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertsieben</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshunderteinundvierzig</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertsieben</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshunderteinundvierzig</t>
         </is>
       </c>
       <c r="D43" t="b">
@@ -1201,16 +1201,16 @@
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>-2147483606</v>
+        <v>2147483642</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertsechs</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertzweiundvierzig</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertsechs</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertzweiundvierzig</t>
         </is>
       </c>
       <c r="D44" t="b">
@@ -1219,16 +1219,16 @@
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>-2147483605</v>
+        <v>2147483643</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertfuenf</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertdreiundvierzig</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertfuenf</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertdreiundvierzig</t>
         </is>
       </c>
       <c r="D45" t="b">
@@ -1237,16 +1237,16 @@
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>-2147483604</v>
+        <v>2147483644</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertvier</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertvierundvierzig</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertvier</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertvierundvierzig</t>
         </is>
       </c>
       <c r="D46" t="b">
@@ -1255,16 +1255,16 @@
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>-2147483603</v>
+        <v>2147483645</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertdrei</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertfuenfundvierzig</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertdrei</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertfuenfundvierzig</t>
         </is>
       </c>
       <c r="D47" t="b">
@@ -1273,16 +1273,16 @@
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>-2147483602</v>
+        <v>2147483646</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertzwei</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertsechsundvierzig</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertzwei</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertsechsundvierzig</t>
         </is>
       </c>
       <c r="D48" t="b">
@@ -1291,16 +1291,16 @@
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>-2147483601</v>
+        <v>2147483647</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshunderteins</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertsiebenundvierzig</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshunderteins</t>
+          <t xml:space="preserve"> zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertsiebenundvierzig</t>
         </is>
       </c>
       <c r="D49" t="b">
@@ -1309,16 +1309,16 @@
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>-2147483600</v>
+        <v>2147483648</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundert</t>
+          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertachtundvierzig</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundert</t>
+          <t xml:space="preserve"> minus zweimilliardeneinhundertsiebenundvierzigmillionenvierhundertdreiundachtzigtausendsechshundertachtundvierzig</t>
         </is>
       </c>
       <c r="D50" t="b">

</xml_diff>